<commit_message>
word to pdf conversion fixed
</commit_message>
<xml_diff>
--- a/src/main/java/files/Data.xlsx
+++ b/src/main/java/files/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IntelliJ\PDFProject_2.0\src\main\java\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CEC714-10B6-41D1-BAAB-8C6573E4B491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B56E4C9-691F-431B-B9C8-4AD0C9E6D503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{65A5DB5C-6C63-41AA-95C1-877B328348E0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>PATH 1</t>
   </si>
@@ -454,8 +454,8 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2">
-        <v>3</v>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>9</v>

</xml_diff>